<commit_message>
Update the inputs for q-learning players
</commit_message>
<xml_diff>
--- a/compare/Compare.xlsx
+++ b/compare/Compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baral\PycharmProjects\ReinforcementLearning\BlackJack\compare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8CBE89-09DF-4020-A8AD-34BBE2294029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5694E883-A2EC-482F-97C7-740BB741066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -103,7 +103,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -142,6 +142,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>STRATEGY</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> COMPARISON </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -228,10 +258,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$I$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$I$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -249,22 +286,23 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>100000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$I$2</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$I$2</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$2:$G$2</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>-4489.5</c:v>
                 </c:pt>
@@ -282,12 +320,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-4548</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-4673.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-4575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -340,10 +372,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$I$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$I$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -361,22 +400,23 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>100000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$I$3</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$3:$I$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$3:$G$3</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>106</c:v>
                 </c:pt>
@@ -394,12 +434,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-131.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>61.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-149.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -452,10 +486,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$I$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$I$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -473,22 +514,23 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>100000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$I$4</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$4:$I$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$4:$G$4</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>161</c:v>
                 </c:pt>
@@ -506,12 +548,6 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-252.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-94</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-113.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -562,10 +598,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$I$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$I$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -583,45 +626,40 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>100000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$I$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$5:$I$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$5:$G$5</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-1435.5</c:v>
+                  <c:v>-1697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1690</c:v>
+                  <c:v>-1983.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1736</c:v>
+                  <c:v>-1999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1464</c:v>
+                  <c:v>-1061</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1460</c:v>
+                  <c:v>-1207</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1442</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1278</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1314</c:v>
+                  <c:v>-1014</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -672,10 +710,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$I$1</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$I$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$1:$G$1</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
@@ -693,45 +738,40 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10000000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>100000000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1000000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$I$6</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$6:$I$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$6:$G$6</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0_ ;_ * \-#,##0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-5000</c:v>
+                  <c:v>-1511</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4138</c:v>
+                  <c:v>-1957</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3591.5</c:v>
+                  <c:v>-1844</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3057</c:v>
+                  <c:v>-1000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1804</c:v>
+                  <c:v>-1084</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1651</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1889</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1673.5</c:v>
+                  <c:v>-941</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -744,7 +784,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1938,10 +1977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1964,7 +2003,7 @@
     <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1989,16 +2028,8 @@
         <f>F1*10</f>
         <v>10000000</v>
       </c>
-      <c r="H1" s="1">
-        <f>G1*10</f>
-        <v>100000000</v>
-      </c>
-      <c r="I1" s="1">
-        <f>H1*10</f>
-        <v>1000000000</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2020,14 +2051,8 @@
       <c r="G2" s="1">
         <v>-4548</v>
       </c>
-      <c r="H2" s="1">
-        <v>-4673.5</v>
-      </c>
-      <c r="I2" s="1">
-        <v>-4575</v>
-      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2049,14 +2074,8 @@
       <c r="G3" s="1">
         <v>-131.5</v>
       </c>
-      <c r="H3" s="1">
-        <v>61.5</v>
-      </c>
-      <c r="I3" s="1">
-        <v>-149.5</v>
-      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2078,69 +2097,51 @@
       <c r="G4" s="1">
         <v>-252.5</v>
       </c>
-      <c r="H4" s="1">
-        <v>-94</v>
-      </c>
-      <c r="I4" s="1">
-        <v>-113.5</v>
-      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>-1435.5</v>
+        <v>-1697</v>
       </c>
       <c r="C5" s="1">
-        <v>-1690</v>
+        <v>-1983.5</v>
       </c>
       <c r="D5" s="1">
-        <v>-1736</v>
+        <v>-1999</v>
       </c>
       <c r="E5" s="1">
-        <v>-1464</v>
+        <v>-1061</v>
       </c>
       <c r="F5" s="1">
-        <v>-1460</v>
+        <v>-1207</v>
       </c>
       <c r="G5" s="1">
-        <v>-1442</v>
-      </c>
-      <c r="H5" s="1">
-        <v>-1278</v>
-      </c>
-      <c r="I5" s="1">
-        <v>-1314</v>
+        <v>-1014</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>-5000</v>
+        <v>-1511</v>
       </c>
       <c r="C6" s="1">
-        <v>-4138</v>
+        <v>-1957</v>
       </c>
       <c r="D6" s="1">
-        <v>-3591.5</v>
+        <v>-1844</v>
       </c>
       <c r="E6" s="1">
-        <v>-3057</v>
+        <v>-1000</v>
       </c>
       <c r="F6" s="1">
-        <v>-1804</v>
+        <v>-1084</v>
       </c>
       <c r="G6" s="1">
-        <v>-1651</v>
-      </c>
-      <c r="H6" s="1">
-        <v>-1889</v>
-      </c>
-      <c r="I6" s="1">
-        <v>-1673.5</v>
+        <v>-941</v>
       </c>
     </row>
   </sheetData>

</xml_diff>